<commit_message>
calculated demand and added shiny figures
</commit_message>
<xml_diff>
--- a/data/genus_ear_wb_age_sex_key.xlsx
+++ b/data/genus_ear_wb_age_sex_key.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrient_endowment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722B3AFE-37B0-C042-BE01-8344F87F68F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD950B7-63AF-1A42-8B58-EFCC21D5AD24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16160" yWindow="6040" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C54852D5-2AE6-7A48-B65C-9FA02C2E1D48}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{C54852D5-2AE6-7A48-B65C-9FA02C2E1D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Nice" sheetId="1" r:id="rId1"/>
-    <sheet name="Useful" sheetId="2" r:id="rId2"/>
+    <sheet name="Useful" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="48">
   <si>
     <t>EAR</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>age_final</t>
+  </si>
+  <si>
+    <t>UN-WPP Popopulation</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>90-94</t>
+  </si>
+  <si>
+    <t>95-99</t>
+  </si>
+  <si>
+    <t>100+</t>
+  </si>
+  <si>
+    <t>age_un</t>
   </si>
 </sst>
 </file>
@@ -221,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -229,8 +250,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EDB1EC-4AD8-CA42-A36F-EEEB3E9538BE}">
-  <dimension ref="A2:K22"/>
+  <dimension ref="A2:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="M3" activeCellId="4" sqref="A3:A26 D3:D26 G3:G26 J3:J26 M3:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,11 +582,14 @@
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -583,11 +606,16 @@
       <c r="H2" s="5"/>
       <c r="I2" s="3"/>
       <c r="J2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -615,8 +643,15 @@
       <c r="K3" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -637,13 +672,19 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -664,13 +705,19 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -691,13 +738,19 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
         <v>34</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -721,10 +774,16 @@
         <v>3</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -750,8 +809,14 @@
       <c r="K8" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -771,14 +836,20 @@
       <c r="H9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -804,8 +875,14 @@
       <c r="K10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -831,8 +908,14 @@
       <c r="K11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -858,8 +941,14 @@
       <c r="K12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -885,8 +974,14 @@
       <c r="K13" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -912,8 +1007,14 @@
       <c r="K14" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -939,8 +1040,14 @@
       <c r="K15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -966,8 +1073,14 @@
       <c r="K16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -993,8 +1106,14 @@
       <c r="K17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1020,8 +1139,14 @@
       <c r="K18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1047,8 +1172,14 @@
       <c r="K19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1074,8 +1205,14 @@
       <c r="K20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1101,8 +1238,14 @@
       <c r="K21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1123,9 +1266,143 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1135,19 +1412,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EFCB0-31EC-7D48-9E4F-6DF6A908A586}">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE29687-4D32-0845-AE85-EFCD6A83DFC4}">
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="6"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1157,273 +1431,401 @@
       <c r="C1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>